<commit_message>
Correct tab name from 'pantallaso' to 'pantallazo'
Correct tab name in Alex's excel files, from 'pantallaso' to 'pantallazo'
</commit_message>
<xml_diff>
--- a/datosAlex/datos2visum.xlsx
+++ b/datosAlex/datos2visum.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\useri3\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MATSim\workspace-mars\dta-brt\datosAlex\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Pantallaso" sheetId="2" r:id="rId2"/>
+    <sheet name="Pantallazo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -5614,7 +5614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:O1228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
@@ -52033,7 +52033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>

</xml_diff>